<commit_message>
added my user stories
</commit_message>
<xml_diff>
--- a/User Stories [TEMPLATE].xlsx
+++ b/User Stories [TEMPLATE].xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\T17-Spint2C4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t xml:space="preserve"> EPIC</t>
   </si>
@@ -79,25 +79,10 @@
     <t>ROW(S)</t>
   </si>
   <si>
-    <t>[Theme, Epic, or Dept]: [High Level Piece of Functionality]</t>
-  </si>
-  <si>
-    <t>As a [archetype], I want to be able to [do a thing], so that I can [achieve a goal]</t>
-  </si>
-  <si>
     <t>1 High</t>
   </si>
   <si>
     <t>LG</t>
-  </si>
-  <si>
-    <t>[A list of acceptance tests]</t>
-  </si>
-  <si>
-    <t>[Any thing that must be done prior to this story]</t>
-  </si>
-  <si>
-    <t>[Who asked for this feature]</t>
   </si>
   <si>
     <t>[Any relevant notes]</t>
@@ -105,12 +90,39 @@
   <si>
     <t xml:space="preserve"> [High Level Piece of Functionality]</t>
   </si>
+  <si>
+    <t>Chat Room</t>
+  </si>
+  <si>
+    <t>Video and Audio icons available for toggling with corresponding actions.</t>
+  </si>
+  <si>
+    <t>As a User , I want to send text meassages in chats in Public Sessions.</t>
+  </si>
+  <si>
+    <t>XXLG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View sent and received messages in session </t>
+  </si>
+  <si>
+    <t>As a User , I want to exit the chat whenever I am done with my questions in Public and Private sessions.</t>
+  </si>
+  <si>
+    <t>As an Expert , I want to have the option to voice call or video call in Public and Private sessions.</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>Finishing the session with a re-direction to the rating bar and feedback template.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -144,6 +156,16 @@
     <font>
       <sz val="8"/>
       <color rgb="FF999999"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF434343"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -230,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -284,6 +306,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -824,15 +855,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="2" width="69.28515625" customWidth="1"/>
+    <col min="2" max="2" width="73.42578125" customWidth="1"/>
     <col min="3" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="8" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" customWidth="1"/>
+    <col min="6" max="8" width="31.140625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
     <col min="10" max="19" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
@@ -896,30 +928,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="22.5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:19" ht="25.5">
+      <c r="A2" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>26</v>
       </c>
       <c r="I2" s="15" t="e">
         <f>IF(AND(OR(#REF!="1 High",#REF!="2 Med"),OR(#REF!="1 High",#REF!="2 Med")),"Strategic",IF(AND(OR(#REF!="1 High",#REF!="2 Med"),OR(#REF!="3 Med",#REF!="4 Low")),"Leveraged",IF(AND(OR(#REF!="3 Med",#REF!="4 Low"),OR(#REF!="1 High",#REF!="2 Med")),"Focused",IF(AND(OR(#REF!="3 Med",#REF!="4 Low"),OR(#REF!="3 Med",#REF!="4 Low")),"Routine",""))))</f>
@@ -954,7 +982,7 @@
         <v>[Theme, Epic, or Dept]</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="R2" s="19" t="e">
         <f t="shared" ref="R2:R1000" si="5">IF(#REF!="MVP","0.0 MVP",#REF!)</f>
@@ -967,17 +995,25 @@
     </row>
     <row r="3" spans="1:19" ht="12.75">
       <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="14"/>
       <c r="I3" s="15"/>
-      <c r="J3" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="J3" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K3" s="17" t="e">
         <f t="shared" ref="K3:L3" si="7">IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -987,9 +1023,9 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="M3" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="M3" s="16">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="N3" s="16" t="e">
         <f t="shared" ref="N3:O3" si="8">IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1008,24 +1044,32 @@
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="S3" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="12.75">
+      <c r="S3" s="20">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="25.5">
       <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
+      <c r="B4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
-      <c r="J4" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="J4" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K4" s="17" t="e">
         <f t="shared" ref="K4:L4" si="9">IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1035,9 +1079,9 @@
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="M4" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="M4" s="16">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="N4" s="16" t="e">
         <f t="shared" ref="N4:O4" si="10">IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1056,9 +1100,9 @@
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="S4" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="S4" s="20">
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="12.75">
@@ -51439,6 +51483,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>